<commit_message>
Analyzed Expenses data a bit
</commit_message>
<xml_diff>
--- a/ExpenseAnalysis/data/Expenses.xlsx
+++ b/ExpenseAnalysis/data/Expenses.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="53">
   <si>
     <t>Remaining Balance</t>
   </si>
@@ -160,9 +160,6 @@
     <t>Iftar</t>
   </si>
   <si>
-    <t>Gadget</t>
-  </si>
-  <si>
     <t>Medical</t>
   </si>
   <si>
@@ -172,12 +169,6 @@
     <t>Tax</t>
   </si>
   <si>
-    <t xml:space="preserve">Meal </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Toiletries </t>
-  </si>
-  <si>
     <t xml:space="preserve">Fare </t>
   </si>
   <si>
@@ -185,15 +176,6 @@
   </si>
   <si>
     <t>Balance</t>
-  </si>
-  <si>
-    <t>Coffee</t>
-  </si>
-  <si>
-    <t>Brealfast</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Snacks </t>
   </si>
   <si>
     <t>Ticket</t>
@@ -1131,7 +1113,7 @@
     </row>
     <row r="11">
       <c r="A11" s="12" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B11" s="12">
         <v>60.0</v>
@@ -1637,7 +1619,7 @@
     </row>
     <row r="57">
       <c r="A57" s="12" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="B57" s="12">
         <v>30.0</v>
@@ -1648,7 +1630,7 @@
     </row>
     <row r="58">
       <c r="A58" s="12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B58" s="12">
         <v>20.0</v>
@@ -1866,7 +1848,7 @@
     </row>
     <row r="12">
       <c r="A12" s="12" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B12" s="12">
         <v>70.0</v>
@@ -2017,7 +1999,7 @@
     </row>
     <row r="14">
       <c r="A14" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B14" s="12">
         <v>50.0</v>
@@ -2215,7 +2197,7 @@
     </row>
     <row r="32">
       <c r="A32" s="12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B32" s="12">
         <v>10.0</v>
@@ -2248,7 +2230,7 @@
     </row>
     <row r="35">
       <c r="A35" s="12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B35" s="12">
         <v>500.0</v>
@@ -2535,7 +2517,7 @@
     </row>
     <row r="61">
       <c r="A61" s="12" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B61" s="12">
         <v>10.0</v>
@@ -2689,7 +2671,7 @@
     </row>
     <row r="75">
       <c r="A75" s="12" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="B75" s="12">
         <v>20.0</v>
@@ -2700,7 +2682,7 @@
     </row>
     <row r="76">
       <c r="A76" s="12" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="B76" s="12">
         <v>20.0</v>
@@ -3170,7 +3152,7 @@
     </row>
     <row r="27">
       <c r="A27" s="12" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B27" s="12">
         <v>40.0</v>
@@ -3247,7 +3229,7 @@
     </row>
     <row r="34">
       <c r="A34" s="12" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="B34" s="12">
         <v>29.0</v>
@@ -3379,7 +3361,7 @@
     </row>
     <row r="46">
       <c r="A46" s="12" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="B46" s="12">
         <v>30.0</v>
@@ -3401,7 +3383,7 @@
     </row>
     <row r="48">
       <c r="A48" s="12" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B48" s="12">
         <v>50.0</v>
@@ -3456,7 +3438,7 @@
     </row>
     <row r="53">
       <c r="A53" s="12" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B53" s="12">
         <v>40.0</v>
@@ -3555,7 +3537,7 @@
     </row>
     <row r="62">
       <c r="A62" s="12" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B62" s="12">
         <v>1200.0</v>
@@ -11957,7 +11939,7 @@
     </row>
     <row r="65">
       <c r="A65" s="12" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="B65" s="12">
         <v>30.0</v>
@@ -12113,7 +12095,7 @@
     </row>
     <row r="78">
       <c r="A78" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B78" s="12">
         <v>1000.0</v>
@@ -12149,7 +12131,7 @@
     </row>
     <row r="81">
       <c r="A81" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B81" s="12">
         <v>500.0</v>
@@ -12708,7 +12690,7 @@
     </row>
     <row r="47">
       <c r="A47" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B47" s="12">
         <v>47.79</v>
@@ -12843,7 +12825,7 @@
     </row>
     <row r="9">
       <c r="A9" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="12">
         <v>4.78</v>
@@ -13777,7 +13759,7 @@
     </row>
     <row r="34">
       <c r="A34" s="12" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="B34" s="12">
         <v>55.0</v>

</xml_diff>

<commit_message>
Created a Pivot Table where Month,Year is column and Items are index, Costs are values
</commit_message>
<xml_diff>
--- a/ExpenseAnalysis/data/Expenses.xlsx
+++ b/ExpenseAnalysis/data/Expenses.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="52">
   <si>
     <t>Remaining Balance</t>
   </si>
@@ -56,6 +56,15 @@
   </si>
   <si>
     <t>Snacks</t>
+  </si>
+  <si>
+    <t>Fare</t>
+  </si>
+  <si>
+    <t>Meal</t>
+  </si>
+  <si>
+    <t>Breakfast</t>
   </si>
   <si>
     <t>Interest Records</t>
@@ -109,16 +118,7 @@
     <t>Gadgets</t>
   </si>
   <si>
-    <t>Breakfast</t>
-  </si>
-  <si>
     <t>Photocopy</t>
-  </si>
-  <si>
-    <t>Fare</t>
-  </si>
-  <si>
-    <t>Meal</t>
   </si>
   <si>
     <t>Treat</t>
@@ -167,9 +167,6 @@
   </si>
   <si>
     <t>Tax</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fare </t>
   </si>
   <si>
     <t>Utility Bill</t>
@@ -622,7 +619,7 @@
       </c>
       <c r="B1" s="2">
         <f>Salary!B1-B2</f>
-        <v>157136.85</v>
+        <v>156392.85</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -636,8 +633,8 @@
         <v>3</v>
       </c>
       <c r="B2" s="5">
-        <f>SUM(B4:B1016)</f>
-        <v>119098.94</v>
+        <f>SUM(B4:B1031)</f>
+        <v>119842.94</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>4</v>
@@ -655,7 +652,7 @@
         <v>✅</v>
       </c>
       <c r="D3" s="7">
-        <v>2034.0</v>
+        <v>1290.0</v>
       </c>
       <c r="E3" s="8">
         <v>155010.85</v>
@@ -709,182 +706,317 @@
         <v>10</v>
       </c>
       <c r="B6" s="12">
+        <v>90.0</v>
+      </c>
+      <c r="C6" s="10">
+        <v>45449.0</v>
+      </c>
+      <c r="D6" s="12"/>
+    </row>
+    <row r="7" ht="15.0" customHeight="1">
+      <c r="A7" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="12">
+        <v>40.0</v>
+      </c>
+      <c r="C7" s="10">
+        <v>45448.0</v>
+      </c>
+      <c r="D7" s="12"/>
+    </row>
+    <row r="8" ht="15.0" customHeight="1">
+      <c r="A8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="12">
+        <v>70.0</v>
+      </c>
+      <c r="C8" s="10">
+        <v>45448.0</v>
+      </c>
+      <c r="D8" s="12"/>
+    </row>
+    <row r="9" ht="15.0" customHeight="1">
+      <c r="A9" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="12">
+        <v>54.0</v>
+      </c>
+      <c r="C9" s="10">
+        <v>45447.0</v>
+      </c>
+      <c r="D9" s="12"/>
+    </row>
+    <row r="10" ht="15.0" customHeight="1">
+      <c r="A10" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="12">
+        <v>20.0</v>
+      </c>
+      <c r="C10" s="10">
+        <v>45447.0</v>
+      </c>
+      <c r="D10" s="12"/>
+    </row>
+    <row r="11" ht="15.0" customHeight="1">
+      <c r="A11" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="12">
+        <v>30.0</v>
+      </c>
+      <c r="C11" s="10">
+        <v>45446.0</v>
+      </c>
+      <c r="D11" s="12"/>
+    </row>
+    <row r="12" ht="15.0" customHeight="1">
+      <c r="A12" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="12">
+        <v>20.0</v>
+      </c>
+      <c r="C12" s="10">
+        <v>45446.0</v>
+      </c>
+      <c r="D12" s="12"/>
+    </row>
+    <row r="13" ht="15.0" customHeight="1">
+      <c r="A13" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="12">
+        <v>30.0</v>
+      </c>
+      <c r="C13" s="10">
+        <v>45446.0</v>
+      </c>
+      <c r="D13" s="12"/>
+    </row>
+    <row r="14" ht="15.0" customHeight="1">
+      <c r="A14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="12">
+        <v>80.0</v>
+      </c>
+      <c r="C14" s="10">
+        <v>45445.0</v>
+      </c>
+      <c r="D14" s="12"/>
+    </row>
+    <row r="15" ht="15.0" customHeight="1">
+      <c r="A15" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="12">
+        <v>55.0</v>
+      </c>
+      <c r="C15" s="10">
+        <v>45445.0</v>
+      </c>
+      <c r="D15" s="12"/>
+    </row>
+    <row r="16" ht="15.0" customHeight="1">
+      <c r="A16" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="12">
+        <v>100.0</v>
+      </c>
+      <c r="C16" s="10">
+        <v>45445.0</v>
+      </c>
+      <c r="D16" s="12"/>
+    </row>
+    <row r="17" ht="15.0" customHeight="1">
+      <c r="A17" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="12">
+        <v>80.0</v>
+      </c>
+      <c r="C17" s="10">
+        <v>45445.0</v>
+      </c>
+      <c r="D17" s="12"/>
+    </row>
+    <row r="18" ht="15.0" customHeight="1">
+      <c r="A18" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="12">
+        <v>40.0</v>
+      </c>
+      <c r="C18" s="10">
+        <v>45445.0</v>
+      </c>
+      <c r="D18" s="12"/>
+    </row>
+    <row r="19" ht="15.0" customHeight="1">
+      <c r="A19" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="12">
+        <v>25.0</v>
+      </c>
+      <c r="C19" s="10">
+        <v>45444.0</v>
+      </c>
+      <c r="D19" s="12"/>
+    </row>
+    <row r="20" ht="15.0" customHeight="1">
+      <c r="A20" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="12">
+        <v>10.0</v>
+      </c>
+      <c r="C20" s="10">
+        <v>45444.0</v>
+      </c>
+      <c r="D20" s="12"/>
+    </row>
+    <row r="21" ht="15.0" customHeight="1">
+      <c r="A21" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="12">
         <v>50.0</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C21" s="10">
         <v>45444.0</v>
       </c>
-      <c r="D6" s="12"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="13"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="14"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="15"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="14"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="13">
+      <c r="D21" s="12"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="13"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="14"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="15"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="14"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="13">
         <v>45413.0</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B24" s="5">
         <f>'May 24'!B2</f>
         <v>10654.16</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="14"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="13">
+      <c r="C24" s="10"/>
+      <c r="D24" s="14"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="13">
         <v>45383.0</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B25" s="5">
         <f>'April 24'!B2</f>
         <v>18530</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="14"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="13">
+      <c r="C25" s="10"/>
+      <c r="D25" s="14"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="13">
         <v>45352.0</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B26" s="5">
         <f>'March 24'!B2</f>
         <v>6479</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="14"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="13">
+      <c r="C26" s="10"/>
+      <c r="D26" s="14"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="13">
         <v>45323.0</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B27" s="5">
         <f>'February 24'!B2</f>
         <v>13290</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="14"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="13">
+      <c r="C27" s="10"/>
+      <c r="D27" s="14"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="13">
         <v>45292.0</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B28" s="5">
         <f>'January 24'!B2</f>
         <v>4747</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="14"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="13">
+      <c r="C28" s="10"/>
+      <c r="D28" s="14"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="13">
         <v>45261.0</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B29" s="5">
         <f>'December 23'!B2</f>
         <v>10982.78</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="14"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="13">
+      <c r="C29" s="10"/>
+      <c r="D29" s="14"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="13">
         <v>45231.0</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B30" s="5">
         <f>'November 23'!B2</f>
         <v>5608</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="13">
+    <row r="31">
+      <c r="A31" s="13">
         <v>45200.0</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B31" s="5">
         <f>'October 23'!B2</f>
         <v>34074</v>
       </c>
-      <c r="C16" s="10"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="13">
+      <c r="C31" s="10"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="13">
         <v>45170.0</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B32" s="5">
         <f>'September 23'!B2</f>
         <v>1490</v>
       </c>
-      <c r="C17" s="10"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="13">
+      <c r="C32" s="10"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="13">
         <v>45139.0</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B33" s="5">
         <f>'August 23'!B2</f>
         <v>7947</v>
       </c>
-      <c r="C18" s="10"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="13">
+      <c r="C33" s="10"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="13">
         <v>45108.0</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B34" s="5">
         <f>'July 23'!B2</f>
         <v>5247</v>
       </c>
-      <c r="C19" s="10"/>
-    </row>
-    <row r="20">
-      <c r="C20" s="10"/>
-    </row>
-    <row r="21">
-      <c r="C21" s="10"/>
-    </row>
-    <row r="22">
-      <c r="C22" s="10"/>
-    </row>
-    <row r="23">
-      <c r="C23" s="10"/>
-    </row>
-    <row r="24">
-      <c r="C24" s="10"/>
-    </row>
-    <row r="25">
-      <c r="C25" s="10"/>
-    </row>
-    <row r="26">
-      <c r="C26" s="10"/>
-    </row>
-    <row r="27">
-      <c r="C27" s="10"/>
-    </row>
-    <row r="28">
-      <c r="C28" s="10"/>
-    </row>
-    <row r="29">
-      <c r="C29" s="10"/>
-    </row>
-    <row r="30">
-      <c r="C30" s="10"/>
-    </row>
-    <row r="31">
-      <c r="C31" s="10"/>
-    </row>
-    <row r="32">
-      <c r="C32" s="10"/>
-    </row>
-    <row r="33">
-      <c r="C33" s="10"/>
-    </row>
-    <row r="34">
       <c r="C34" s="10"/>
     </row>
     <row r="35">
@@ -964,7 +1096,6 @@
     </row>
     <row r="60">
       <c r="C60" s="10"/>
-      <c r="D60" s="18"/>
     </row>
     <row r="61">
       <c r="C61" s="10"/>
@@ -1006,10 +1137,56 @@
       <c r="C73" s="10"/>
     </row>
     <row r="74">
-      <c r="C74" s="19"/>
+      <c r="C74" s="10"/>
     </row>
     <row r="75">
-      <c r="C75" s="19"/>
+      <c r="C75" s="10"/>
+      <c r="D75" s="18"/>
+    </row>
+    <row r="76">
+      <c r="C76" s="10"/>
+    </row>
+    <row r="77">
+      <c r="C77" s="10"/>
+    </row>
+    <row r="78">
+      <c r="C78" s="10"/>
+    </row>
+    <row r="79">
+      <c r="C79" s="10"/>
+    </row>
+    <row r="80">
+      <c r="C80" s="10"/>
+    </row>
+    <row r="81">
+      <c r="C81" s="10"/>
+    </row>
+    <row r="82">
+      <c r="C82" s="10"/>
+    </row>
+    <row r="83">
+      <c r="C83" s="10"/>
+    </row>
+    <row r="84">
+      <c r="C84" s="10"/>
+    </row>
+    <row r="85">
+      <c r="C85" s="10"/>
+    </row>
+    <row r="86">
+      <c r="C86" s="10"/>
+    </row>
+    <row r="87">
+      <c r="C87" s="10"/>
+    </row>
+    <row r="88">
+      <c r="C88" s="10"/>
+    </row>
+    <row r="89">
+      <c r="C89" s="19"/>
+    </row>
+    <row r="90">
+      <c r="C90" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1080,7 +1257,7 @@
     </row>
     <row r="8">
       <c r="A8" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B8" s="12">
         <v>40.0</v>
@@ -1124,7 +1301,7 @@
     </row>
     <row r="12">
       <c r="A12" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B12" s="12">
         <v>30.0</v>
@@ -1146,7 +1323,7 @@
     </row>
     <row r="14">
       <c r="A14" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B14" s="12">
         <v>20.0</v>
@@ -1157,7 +1334,7 @@
     </row>
     <row r="15">
       <c r="A15" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B15" s="12">
         <v>30.0</v>
@@ -1212,7 +1389,7 @@
     </row>
     <row r="20">
       <c r="A20" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B20" s="12">
         <v>30.0</v>
@@ -1245,7 +1422,7 @@
     </row>
     <row r="23">
       <c r="A23" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B23" s="12">
         <v>25.0</v>
@@ -1278,7 +1455,7 @@
     </row>
     <row r="26">
       <c r="A26" s="12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B26" s="12">
         <v>29500.0</v>
@@ -1300,7 +1477,7 @@
     </row>
     <row r="28">
       <c r="A28" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B28" s="12">
         <v>10.0</v>
@@ -1344,7 +1521,7 @@
     </row>
     <row r="32">
       <c r="A32" s="12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B32" s="12">
         <v>30.0</v>
@@ -1355,7 +1532,7 @@
     </row>
     <row r="33">
       <c r="A33" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B33" s="12">
         <v>30.0</v>
@@ -1399,7 +1576,7 @@
     </row>
     <row r="37">
       <c r="A37" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B37" s="12">
         <v>30.0</v>
@@ -1443,7 +1620,7 @@
     </row>
     <row r="41">
       <c r="A41" s="12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B41" s="12">
         <v>230.0</v>
@@ -1454,7 +1631,7 @@
     </row>
     <row r="42">
       <c r="A42" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B42" s="12">
         <v>10.0</v>
@@ -1553,7 +1730,7 @@
     </row>
     <row r="51">
       <c r="A51" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B51" s="12">
         <v>33.0</v>
@@ -1575,7 +1752,7 @@
     </row>
     <row r="53">
       <c r="A53" s="12" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B53" s="12">
         <v>45.0</v>
@@ -1597,7 +1774,7 @@
     </row>
     <row r="55">
       <c r="A55" s="12" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B55" s="12">
         <v>45.0</v>
@@ -1608,7 +1785,7 @@
     </row>
     <row r="56">
       <c r="A56" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B56" s="12">
         <v>20.0</v>
@@ -1619,7 +1796,7 @@
     </row>
     <row r="57">
       <c r="A57" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B57" s="12">
         <v>30.0</v>
@@ -1630,7 +1807,7 @@
     </row>
     <row r="58">
       <c r="A58" s="12" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="B58" s="12">
         <v>20.0</v>
@@ -1674,7 +1851,7 @@
     </row>
     <row r="62">
       <c r="A62" s="12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B62" s="12">
         <v>10.0</v>
@@ -1955,7 +2132,7 @@
     </row>
     <row r="10">
       <c r="A10" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B10" s="12">
         <v>320.0</v>
@@ -1966,7 +2143,7 @@
     </row>
     <row r="11">
       <c r="A11" s="12" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B11" s="12">
         <v>90.0</v>
@@ -1977,7 +2154,7 @@
     </row>
     <row r="12">
       <c r="A12" s="12" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B12" s="12">
         <v>55.0</v>
@@ -1988,7 +2165,7 @@
     </row>
     <row r="13">
       <c r="A13" s="12" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B13" s="12">
         <v>88.0</v>
@@ -1999,13 +2176,13 @@
     </row>
     <row r="14">
       <c r="A14" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B14" s="12">
         <v>50.0</v>
       </c>
       <c r="C14" s="10">
-        <v>44798.0</v>
+        <v>45163.0</v>
       </c>
     </row>
     <row r="15">
@@ -2016,7 +2193,7 @@
         <v>250.0</v>
       </c>
       <c r="C15" s="10">
-        <v>44798.0</v>
+        <v>45163.0</v>
       </c>
     </row>
     <row r="16">
@@ -2032,7 +2209,7 @@
     </row>
     <row r="17">
       <c r="A17" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B17" s="12">
         <v>30.0</v>
@@ -2076,7 +2253,7 @@
     </row>
     <row r="21">
       <c r="A21" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B21" s="12">
         <v>45.0</v>
@@ -2109,7 +2286,7 @@
     </row>
     <row r="24">
       <c r="A24" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B24" s="12">
         <v>30.0</v>
@@ -2142,7 +2319,7 @@
     </row>
     <row r="27">
       <c r="A27" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B27" s="12">
         <v>30.0</v>
@@ -2175,7 +2352,7 @@
     </row>
     <row r="30">
       <c r="A30" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B30" s="12">
         <v>30.0</v>
@@ -2197,7 +2374,7 @@
     </row>
     <row r="32">
       <c r="A32" s="12" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="B32" s="12">
         <v>10.0</v>
@@ -2230,7 +2407,7 @@
     </row>
     <row r="35">
       <c r="A35" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B35" s="12">
         <v>500.0</v>
@@ -2242,7 +2419,7 @@
     </row>
     <row r="36">
       <c r="A36" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B36" s="12">
         <v>35.0</v>
@@ -2264,7 +2441,7 @@
     </row>
     <row r="38">
       <c r="A38" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B38" s="12">
         <v>35.0</v>
@@ -2330,7 +2507,7 @@
     </row>
     <row r="44">
       <c r="A44" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B44" s="12">
         <v>30.0</v>
@@ -2352,7 +2529,7 @@
     </row>
     <row r="46">
       <c r="A46" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B46" s="12">
         <v>25.0</v>
@@ -2385,7 +2562,7 @@
     </row>
     <row r="49">
       <c r="A49" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B49" s="12">
         <v>33.0</v>
@@ -2396,7 +2573,7 @@
     </row>
     <row r="50">
       <c r="A50" s="12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B50" s="12">
         <v>10.0</v>
@@ -2407,7 +2584,7 @@
     </row>
     <row r="51">
       <c r="A51" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B51" s="12">
         <v>20.0</v>
@@ -2429,7 +2606,7 @@
     </row>
     <row r="53">
       <c r="A53" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B53" s="12">
         <v>29.0</v>
@@ -2462,7 +2639,7 @@
     </row>
     <row r="56">
       <c r="A56" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B56" s="12">
         <v>25.0</v>
@@ -2473,7 +2650,7 @@
     </row>
     <row r="57">
       <c r="A57" s="12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B57" s="12">
         <v>710.0</v>
@@ -2495,7 +2672,7 @@
     </row>
     <row r="59">
       <c r="A59" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B59" s="12">
         <v>29.0</v>
@@ -2539,7 +2716,7 @@
     </row>
     <row r="63">
       <c r="A63" s="12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B63" s="12">
         <v>30.0</v>
@@ -2561,7 +2738,7 @@
     </row>
     <row r="65">
       <c r="A65" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B65" s="12">
         <v>30.0</v>
@@ -2594,7 +2771,7 @@
     </row>
     <row r="68">
       <c r="A68" s="12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B68" s="12">
         <v>4.0</v>
@@ -2616,7 +2793,7 @@
     </row>
     <row r="70">
       <c r="A70" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B70" s="12">
         <v>29.0</v>
@@ -2638,7 +2815,7 @@
     </row>
     <row r="72">
       <c r="A72" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B72" s="12">
         <v>29.0</v>
@@ -2649,7 +2826,7 @@
     </row>
     <row r="73">
       <c r="A73" s="12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B73" s="12">
         <v>2.0</v>
@@ -2660,7 +2837,7 @@
     </row>
     <row r="74">
       <c r="A74" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B74" s="12">
         <v>29.0</v>
@@ -2726,7 +2903,7 @@
     </row>
     <row r="80">
       <c r="A80" s="12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B80" s="12">
         <v>30.0</v>
@@ -2803,7 +2980,7 @@
     </row>
     <row r="87">
       <c r="A87" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B87" s="12">
         <v>29.0</v>
@@ -2825,7 +3002,7 @@
     </row>
     <row r="89">
       <c r="A89" s="12" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B89" s="12">
         <v>45.0</v>
@@ -2836,7 +3013,7 @@
     </row>
     <row r="90">
       <c r="A90" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B90" s="12">
         <v>29.0</v>
@@ -2847,7 +3024,7 @@
     </row>
     <row r="91">
       <c r="A91" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B91" s="12">
         <v>29.0</v>
@@ -2921,7 +3098,7 @@
     </row>
     <row r="6">
       <c r="A6" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B6" s="12">
         <v>29.0</v>
@@ -2954,7 +3131,7 @@
     </row>
     <row r="9">
       <c r="A9" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B9" s="12">
         <v>34.0</v>
@@ -2987,7 +3164,7 @@
     </row>
     <row r="12">
       <c r="A12" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B12" s="12">
         <v>29.0</v>
@@ -3020,7 +3197,7 @@
     </row>
     <row r="15">
       <c r="A15" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B15" s="12">
         <v>34.0</v>
@@ -3031,7 +3208,7 @@
     </row>
     <row r="16">
       <c r="A16" s="12" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B16" s="12">
         <v>47.0</v>
@@ -3042,7 +3219,7 @@
     </row>
     <row r="17">
       <c r="A17" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B17" s="12">
         <v>10.0</v>
@@ -3053,7 +3230,7 @@
     </row>
     <row r="18">
       <c r="A18" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B18" s="12">
         <v>30.0</v>
@@ -3064,7 +3241,7 @@
     </row>
     <row r="19">
       <c r="A19" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B19" s="12">
         <v>80.0</v>
@@ -3086,7 +3263,7 @@
     </row>
     <row r="21">
       <c r="A21" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B21" s="12">
         <v>30.0</v>
@@ -3119,7 +3296,7 @@
     </row>
     <row r="24">
       <c r="A24" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B24" s="12">
         <v>20.0</v>
@@ -3163,7 +3340,7 @@
     </row>
     <row r="28">
       <c r="A28" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B28" s="12">
         <v>34.0</v>
@@ -3185,7 +3362,7 @@
     </row>
     <row r="30">
       <c r="A30" s="12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B30" s="12">
         <v>15.0</v>
@@ -3229,7 +3406,7 @@
     </row>
     <row r="34">
       <c r="A34" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B34" s="12">
         <v>29.0</v>
@@ -3262,7 +3439,7 @@
     </row>
     <row r="37">
       <c r="A37" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B37" s="12">
         <v>30.0</v>
@@ -3284,7 +3461,7 @@
     </row>
     <row r="39">
       <c r="A39" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B39" s="12">
         <v>34.0</v>
@@ -3317,7 +3494,7 @@
     </row>
     <row r="42">
       <c r="A42" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B42" s="12">
         <v>33.0</v>
@@ -3350,7 +3527,7 @@
     </row>
     <row r="45">
       <c r="A45" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B45" s="12">
         <v>20.0</v>
@@ -3383,7 +3560,7 @@
     </row>
     <row r="48">
       <c r="A48" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B48" s="12">
         <v>50.0</v>
@@ -3405,7 +3582,7 @@
     </row>
     <row r="50">
       <c r="A50" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B50" s="12">
         <v>30.0</v>
@@ -3416,7 +3593,7 @@
     </row>
     <row r="51">
       <c r="A51" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B51" s="12">
         <v>30.0</v>
@@ -3449,7 +3626,7 @@
     </row>
     <row r="54">
       <c r="A54" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B54" s="12">
         <v>20.0</v>
@@ -3460,7 +3637,7 @@
     </row>
     <row r="55">
       <c r="A55" s="12" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B55" s="12">
         <v>120.0</v>
@@ -3482,7 +3659,7 @@
     </row>
     <row r="57">
       <c r="A57" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B57" s="12">
         <v>29.0</v>
@@ -3504,7 +3681,7 @@
     </row>
     <row r="59">
       <c r="A59" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B59" s="12">
         <v>45.0</v>
@@ -3537,7 +3714,7 @@
     </row>
     <row r="62">
       <c r="A62" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B62" s="12">
         <v>1200.0</v>
@@ -3608,7 +3785,7 @@
       <c r="C2" s="21"/>
       <c r="D2" s="11"/>
       <c r="E2" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H2" s="21"/>
       <c r="I2" s="21"/>
@@ -3635,29 +3812,29 @@
         <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
       <c r="M3" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="O3" s="11"/>
       <c r="P3" s="11"/>
@@ -3680,7 +3857,7 @@
         <v>7040.0</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D4" s="23"/>
       <c r="E4" s="12">
@@ -3710,7 +3887,7 @@
         <v>7031.0</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D5" s="23"/>
       <c r="I5" s="12" t="s">
@@ -3720,10 +3897,10 @@
         <v>320.0</v>
       </c>
       <c r="M5" s="24" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="N5" s="25" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6">
@@ -3734,20 +3911,20 @@
         <v>15000.0</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D6" s="23"/>
       <c r="I6" s="12" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="J6" s="12">
         <v>40.0</v>
       </c>
       <c r="M6" s="24" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="N6" s="25" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7">
@@ -3758,11 +3935,11 @@
         <v>7012.0</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D7" s="23"/>
       <c r="I7" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="J7" s="12">
         <v>175.0</v>
@@ -3777,7 +3954,7 @@
         <v>15000.0</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D8" s="23"/>
       <c r="N8" s="26"/>
@@ -3790,7 +3967,7 @@
         <v>7055.0</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D9" s="23"/>
       <c r="N9" s="26"/>
@@ -3803,7 +3980,7 @@
         <v>15000.0</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D10" s="23"/>
       <c r="N10" s="26"/>
@@ -3816,7 +3993,7 @@
         <v>7288.0</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D11" s="23"/>
       <c r="N11" s="26"/>
@@ -3829,7 +4006,7 @@
         <v>22000.0</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D12" s="23"/>
       <c r="N12" s="26"/>
@@ -3842,7 +4019,7 @@
         <v>7262.0</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D13" s="23"/>
       <c r="N13" s="26"/>
@@ -3855,7 +4032,7 @@
         <v>22000.0</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D14" s="23"/>
       <c r="N14" s="26"/>
@@ -3868,7 +4045,7 @@
         <v>22000.0</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D15" s="23"/>
       <c r="N15" s="26"/>
@@ -3881,10 +4058,10 @@
         <v>14500.0</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="N16" s="26"/>
     </row>
@@ -3896,7 +4073,7 @@
         <v>22000.0</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D17" s="23"/>
       <c r="N17" s="26"/>
@@ -3909,10 +4086,10 @@
         <v>10000.0</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="N18" s="26"/>
     </row>
@@ -3924,7 +4101,7 @@
         <v>22000.0</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="N19" s="26"/>
     </row>
@@ -3936,7 +4113,7 @@
         <v>22000.0</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D20" s="23"/>
       <c r="N20" s="26"/>
@@ -3949,10 +4126,10 @@
         <v>10000.0</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="N21" s="26"/>
     </row>
@@ -3964,7 +4141,7 @@
         <v>22000.0</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F22" s="27"/>
       <c r="N22" s="26"/>
@@ -7940,7 +8117,7 @@
     </row>
     <row r="6">
       <c r="A6" s="12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B6" s="12">
         <v>30.0</v>
@@ -7964,7 +8141,7 @@
     </row>
     <row r="8">
       <c r="A8" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B8" s="12">
         <v>30.0</v>
@@ -8000,7 +8177,7 @@
     </row>
     <row r="11">
       <c r="A11" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B11" s="12">
         <v>20.0</v>
@@ -8060,7 +8237,7 @@
     </row>
     <row r="16">
       <c r="A16" s="12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B16" s="12">
         <v>6.0</v>
@@ -8072,7 +8249,7 @@
     </row>
     <row r="17">
       <c r="A17" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B17" s="12">
         <v>605.0</v>
@@ -8096,7 +8273,7 @@
     </row>
     <row r="19">
       <c r="A19" s="12" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B19" s="12">
         <v>40.0</v>
@@ -8180,7 +8357,7 @@
     </row>
     <row r="26">
       <c r="A26" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B26" s="12">
         <v>30.0</v>
@@ -8192,7 +8369,7 @@
     </row>
     <row r="27">
       <c r="A27" s="12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B27" s="12">
         <v>385.0</v>
@@ -8204,7 +8381,7 @@
     </row>
     <row r="28">
       <c r="A28" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B28" s="12">
         <v>20.0</v>
@@ -8288,7 +8465,7 @@
     </row>
     <row r="35">
       <c r="A35" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B35" s="12">
         <v>30.0</v>
@@ -8312,7 +8489,7 @@
     </row>
     <row r="37">
       <c r="A37" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B37" s="12">
         <v>30.0</v>
@@ -8348,7 +8525,7 @@
     </row>
     <row r="40">
       <c r="A40" s="12" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B40" s="12">
         <v>115.0</v>
@@ -8384,7 +8561,7 @@
     </row>
     <row r="43">
       <c r="A43" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B43" s="12">
         <v>15.0</v>
@@ -8396,7 +8573,7 @@
     </row>
     <row r="44">
       <c r="A44" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B44" s="12">
         <v>30.0</v>
@@ -8420,7 +8597,7 @@
     </row>
     <row r="46">
       <c r="A46" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B46" s="12">
         <v>30.0</v>
@@ -8504,7 +8681,7 @@
     </row>
     <row r="53">
       <c r="A53" s="12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B53" s="12">
         <v>30.0</v>
@@ -8588,7 +8765,7 @@
     </row>
     <row r="60">
       <c r="A60" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B60" s="12">
         <v>30.0</v>
@@ -8636,7 +8813,7 @@
     </row>
     <row r="64">
       <c r="A64" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B64" s="12">
         <v>30.0</v>
@@ -8684,7 +8861,7 @@
     </row>
     <row r="68">
       <c r="A68" s="12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B68" s="12">
         <v>610.0</v>
@@ -8732,7 +8909,7 @@
     </row>
     <row r="72">
       <c r="A72" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B72" s="12">
         <v>25.0</v>
@@ -8780,7 +8957,7 @@
     </row>
     <row r="76">
       <c r="A76" s="12" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B76" s="12">
         <v>55.0</v>
@@ -8792,7 +8969,7 @@
     </row>
     <row r="77">
       <c r="A77" s="12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B77" s="12">
         <v>133.0</v>
@@ -8816,7 +8993,7 @@
     </row>
     <row r="79">
       <c r="A79" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B79" s="12">
         <v>40.0</v>
@@ -8876,7 +9053,7 @@
     </row>
     <row r="84">
       <c r="A84" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B84" s="12">
         <v>20.0</v>
@@ -8888,7 +9065,7 @@
     </row>
     <row r="85">
       <c r="A85" s="12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B85" s="12">
         <v>380.0</v>
@@ -8912,7 +9089,7 @@
     </row>
     <row r="87">
       <c r="A87" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B87" s="12">
         <v>5.0</v>
@@ -9032,7 +9209,7 @@
     </row>
     <row r="97">
       <c r="A97" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B97" s="12">
         <v>40.0</v>
@@ -9092,7 +9269,7 @@
     </row>
     <row r="102">
       <c r="A102" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B102" s="12">
         <v>30.0</v>
@@ -9116,7 +9293,7 @@
     </row>
     <row r="104">
       <c r="A104" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B104" s="12">
         <v>40.0</v>
@@ -9140,7 +9317,7 @@
     </row>
     <row r="106">
       <c r="A106" s="12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B106" s="12">
         <v>6.0</v>
@@ -9176,7 +9353,7 @@
     </row>
     <row r="109">
       <c r="A109" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B109" s="12">
         <v>10.0</v>
@@ -9200,7 +9377,7 @@
     </row>
     <row r="111">
       <c r="A111" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B111" s="12">
         <v>10.0</v>
@@ -9236,7 +9413,7 @@
     </row>
     <row r="114">
       <c r="A114" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B114" s="12">
         <v>40.0</v>
@@ -9339,7 +9516,7 @@
     </row>
     <row r="6">
       <c r="A6" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B6" s="12">
         <v>30.0</v>
@@ -9387,7 +9564,7 @@
     </row>
     <row r="10">
       <c r="A10" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B10" s="12">
         <v>30.0</v>
@@ -9423,7 +9600,7 @@
     </row>
     <row r="13">
       <c r="A13" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B13" s="12">
         <v>30.0</v>
@@ -9447,7 +9624,7 @@
     </row>
     <row r="15">
       <c r="A15" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B15" s="12">
         <v>30.0</v>
@@ -9471,7 +9648,7 @@
     </row>
     <row r="17">
       <c r="A17" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B17" s="12">
         <v>30.0</v>
@@ -9507,7 +9684,7 @@
     </row>
     <row r="20">
       <c r="A20" s="12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B20" s="12">
         <v>60.0</v>
@@ -9531,7 +9708,7 @@
     </row>
     <row r="22">
       <c r="A22" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B22" s="12">
         <v>140.0</v>
@@ -9543,7 +9720,7 @@
     </row>
     <row r="23">
       <c r="A23" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B23" s="12">
         <v>30.0</v>
@@ -9579,7 +9756,7 @@
     </row>
     <row r="26">
       <c r="A26" s="12" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B26" s="12">
         <v>150.0</v>
@@ -9615,7 +9792,7 @@
     </row>
     <row r="29">
       <c r="A29" s="12" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B29" s="12">
         <v>45.0</v>
@@ -9639,7 +9816,7 @@
     </row>
     <row r="31">
       <c r="A31" s="12" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B31" s="12">
         <v>45.0</v>
@@ -9663,7 +9840,7 @@
     </row>
     <row r="33">
       <c r="A33" s="12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B33" s="12">
         <v>5.0</v>
@@ -9699,7 +9876,7 @@
     </row>
     <row r="36">
       <c r="A36" s="12" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B36" s="12">
         <v>45.0</v>
@@ -9711,7 +9888,7 @@
     </row>
     <row r="37">
       <c r="A37" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B37" s="12">
         <v>20.0</v>
@@ -9758,7 +9935,7 @@
     </row>
     <row r="41">
       <c r="A41" s="12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B41" s="12">
         <v>150.0</v>
@@ -9770,7 +9947,7 @@
     </row>
     <row r="42">
       <c r="A42" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B42" s="12">
         <v>25.0</v>
@@ -9818,7 +9995,7 @@
     </row>
     <row r="46">
       <c r="A46" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B46" s="12">
         <v>60.0</v>
@@ -9865,7 +10042,7 @@
     </row>
     <row r="50">
       <c r="A50" s="12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B50" s="12">
         <v>30.0</v>
@@ -9901,7 +10078,7 @@
     </row>
     <row r="53">
       <c r="A53" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B53" s="12">
         <v>20.0</v>
@@ -9997,7 +10174,7 @@
     </row>
     <row r="61">
       <c r="A61" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B61" s="12">
         <v>800.0</v>
@@ -10009,7 +10186,7 @@
     </row>
     <row r="62">
       <c r="A62" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B62" s="12">
         <v>10.0</v>
@@ -10057,7 +10234,7 @@
     </row>
     <row r="66">
       <c r="A66" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B66" s="12">
         <v>10.0</v>
@@ -10189,7 +10366,7 @@
     </row>
     <row r="77">
       <c r="A77" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B77" s="12">
         <v>40.0</v>
@@ -10376,7 +10553,7 @@
     </row>
     <row r="10">
       <c r="A10" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B10" s="12">
         <v>130.0</v>
@@ -10400,7 +10577,7 @@
     </row>
     <row r="12">
       <c r="A12" s="12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B12" s="12">
         <v>2.0</v>
@@ -10496,7 +10673,7 @@
     </row>
     <row r="20">
       <c r="A20" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B20" s="12">
         <v>60.0</v>
@@ -10580,7 +10757,7 @@
     </row>
     <row r="27">
       <c r="A27" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B27" s="12">
         <v>20.0</v>
@@ -10616,7 +10793,7 @@
     </row>
     <row r="30">
       <c r="A30" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B30" s="12">
         <v>525.0</v>
@@ -10736,7 +10913,7 @@
     </row>
     <row r="40">
       <c r="A40" s="12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B40" s="12">
         <v>30.0</v>
@@ -10820,7 +10997,7 @@
     </row>
     <row r="47">
       <c r="A47" s="12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B47" s="12">
         <v>20.0</v>
@@ -10844,7 +11021,7 @@
     </row>
     <row r="49">
       <c r="A49" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B49" s="12">
         <v>30.0</v>
@@ -10868,7 +11045,7 @@
     </row>
     <row r="51">
       <c r="A51" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B51" s="12">
         <v>30.0</v>
@@ -10916,7 +11093,7 @@
     </row>
     <row r="55">
       <c r="A55" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B55" s="12">
         <v>25.0</v>
@@ -10928,7 +11105,7 @@
     </row>
     <row r="56">
       <c r="A56" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B56" s="12">
         <v>30.0</v>
@@ -10964,7 +11141,7 @@
     </row>
     <row r="59">
       <c r="A59" s="12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B59" s="12">
         <v>5.0</v>
@@ -10988,7 +11165,7 @@
     </row>
     <row r="61">
       <c r="A61" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B61" s="12">
         <v>30.0</v>
@@ -11060,7 +11237,7 @@
     </row>
     <row r="67">
       <c r="A67" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B67" s="12">
         <v>30.0</v>
@@ -11084,7 +11261,7 @@
     </row>
     <row r="69">
       <c r="A69" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B69" s="12">
         <v>30.0</v>
@@ -11120,7 +11297,7 @@
     </row>
     <row r="72">
       <c r="A72" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B72" s="12">
         <v>30.0</v>
@@ -11144,7 +11321,7 @@
     </row>
     <row r="74">
       <c r="A74" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B74" s="12">
         <v>30.0</v>
@@ -11244,7 +11421,7 @@
     </row>
     <row r="7">
       <c r="A7" s="12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B7" s="12">
         <v>160.0</v>
@@ -11256,7 +11433,7 @@
     </row>
     <row r="8">
       <c r="A8" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B8" s="12">
         <v>30.0</v>
@@ -11280,7 +11457,7 @@
     </row>
     <row r="10">
       <c r="A10" s="12" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B10" s="12">
         <v>45.0</v>
@@ -11316,7 +11493,7 @@
     </row>
     <row r="13">
       <c r="A13" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B13" s="12">
         <v>30.0</v>
@@ -11340,7 +11517,7 @@
     </row>
     <row r="15">
       <c r="A15" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B15" s="12">
         <v>40.0</v>
@@ -11376,7 +11553,7 @@
     </row>
     <row r="18">
       <c r="A18" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B18" s="12">
         <v>30.0</v>
@@ -11424,7 +11601,7 @@
     </row>
     <row r="22">
       <c r="A22" s="12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B22" s="12">
         <v>210.0</v>
@@ -11436,7 +11613,7 @@
     </row>
     <row r="23">
       <c r="A23" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B23" s="12">
         <v>40.0</v>
@@ -11472,7 +11649,7 @@
     </row>
     <row r="26">
       <c r="A26" s="12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B26" s="12">
         <v>425.0</v>
@@ -11508,7 +11685,7 @@
     </row>
     <row r="29">
       <c r="A29" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B29" s="12">
         <v>40.0</v>
@@ -11532,7 +11709,7 @@
     </row>
     <row r="31">
       <c r="A31" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B31" s="12">
         <v>80.0</v>
@@ -11544,7 +11721,7 @@
     </row>
     <row r="32">
       <c r="A32" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B32" s="12">
         <v>30.0</v>
@@ -11580,7 +11757,7 @@
     </row>
     <row r="35">
       <c r="A35" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B35" s="12">
         <v>30.0</v>
@@ -11640,7 +11817,7 @@
     </row>
     <row r="40">
       <c r="A40" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B40" s="12">
         <v>30.0</v>
@@ -11664,7 +11841,7 @@
     </row>
     <row r="42">
       <c r="A42" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B42" s="12">
         <v>20.0</v>
@@ -11723,7 +11900,7 @@
     </row>
     <row r="47">
       <c r="A47" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B47" s="12">
         <v>25.0</v>
@@ -11747,7 +11924,7 @@
     </row>
     <row r="49">
       <c r="A49" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B49" s="12">
         <v>25.0</v>
@@ -11783,7 +11960,7 @@
     </row>
     <row r="52">
       <c r="A52" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B52" s="12">
         <v>30.0</v>
@@ -11843,7 +12020,7 @@
     </row>
     <row r="57">
       <c r="A57" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B57" s="12">
         <v>25.0</v>
@@ -11867,7 +12044,7 @@
     </row>
     <row r="59">
       <c r="A59" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B59" s="12">
         <v>30.0</v>
@@ -11927,7 +12104,7 @@
     </row>
     <row r="64">
       <c r="A64" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B64" s="12">
         <v>25.0</v>
@@ -11939,7 +12116,7 @@
     </row>
     <row r="65">
       <c r="A65" s="12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B65" s="12">
         <v>30.0</v>
@@ -11963,7 +12140,7 @@
     </row>
     <row r="67">
       <c r="A67" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B67" s="12">
         <v>30.0</v>
@@ -11987,7 +12164,7 @@
     </row>
     <row r="69">
       <c r="A69" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B69" s="12">
         <v>30.0</v>
@@ -12035,7 +12212,7 @@
     </row>
     <row r="73">
       <c r="A73" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B73" s="12">
         <v>30.0</v>
@@ -12071,7 +12248,7 @@
     </row>
     <row r="76">
       <c r="A76" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B76" s="12">
         <v>20.0</v>
@@ -12119,7 +12296,7 @@
     </row>
     <row r="80">
       <c r="A80" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B80" s="12">
         <v>800.0</v>
@@ -12143,7 +12320,7 @@
     </row>
     <row r="82">
       <c r="A82" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B82" s="12">
         <v>20.0</v>
@@ -12198,7 +12375,7 @@
     </row>
     <row r="6">
       <c r="A6" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B6" s="12">
         <v>10.0</v>
@@ -12282,7 +12459,7 @@
     </row>
     <row r="13">
       <c r="A13" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B13" s="12">
         <v>30.0</v>
@@ -12498,7 +12675,7 @@
     </row>
     <row r="31">
       <c r="A31" s="12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B31" s="12">
         <v>300.0</v>
@@ -12510,7 +12687,7 @@
     </row>
     <row r="32">
       <c r="A32" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B32" s="12">
         <v>40.0</v>
@@ -12558,7 +12735,7 @@
     </row>
     <row r="36">
       <c r="A36" s="12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B36" s="12">
         <v>600.0</v>
@@ -12570,7 +12747,7 @@
     </row>
     <row r="37">
       <c r="A37" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B37" s="12">
         <v>20.0</v>
@@ -12630,7 +12807,7 @@
     </row>
     <row r="42">
       <c r="A42" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B42" s="12">
         <v>40.0</v>
@@ -12957,7 +13134,7 @@
     </row>
     <row r="20">
       <c r="A20" s="12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B20" s="12">
         <v>314.0</v>
@@ -12981,7 +13158,7 @@
     </row>
     <row r="22">
       <c r="A22" s="12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B22" s="12">
         <v>140.0</v>
@@ -12993,7 +13170,7 @@
     </row>
     <row r="23">
       <c r="A23" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B23" s="12">
         <v>20.0</v>
@@ -13125,7 +13302,7 @@
     </row>
     <row r="34">
       <c r="A34" s="12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B34" s="12">
         <v>776.0</v>
@@ -13161,7 +13338,7 @@
     </row>
     <row r="37">
       <c r="A37" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B37" s="12">
         <v>20.0</v>
@@ -13185,7 +13362,7 @@
     </row>
     <row r="39">
       <c r="A39" s="12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B39" s="12">
         <v>930.0</v>
@@ -13221,7 +13398,7 @@
     </row>
     <row r="42">
       <c r="A42" s="12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B42" s="12">
         <v>30.0</v>
@@ -13257,7 +13434,7 @@
     </row>
     <row r="45">
       <c r="A45" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B45" s="12">
         <v>20.0</v>
@@ -13281,7 +13458,7 @@
     </row>
     <row r="47">
       <c r="A47" s="12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B47" s="12">
         <v>520.0</v>
@@ -13305,7 +13482,7 @@
     </row>
     <row r="49">
       <c r="A49" s="12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B49" s="12">
         <v>999.0</v>
@@ -13317,7 +13494,7 @@
     </row>
     <row r="50">
       <c r="A50" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B50" s="12">
         <v>20.0</v>
@@ -13364,7 +13541,7 @@
     </row>
     <row r="54">
       <c r="A54" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B54" s="12">
         <v>25.0</v>
@@ -13503,7 +13680,7 @@
     </row>
     <row r="11">
       <c r="A11" s="12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B11" s="12">
         <v>884.0</v>
@@ -13550,7 +13727,7 @@
     </row>
     <row r="15">
       <c r="A15" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B15" s="12">
         <v>25.0</v>
@@ -13572,7 +13749,7 @@
     </row>
     <row r="17">
       <c r="A17" s="12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B17" s="12">
         <v>36.0</v>
@@ -13583,7 +13760,7 @@
     </row>
     <row r="18">
       <c r="A18" s="12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B18" s="12">
         <v>550.0</v>
@@ -13594,7 +13771,7 @@
     </row>
     <row r="19">
       <c r="A19" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B19" s="12">
         <v>25.0</v>
@@ -13649,7 +13826,7 @@
     </row>
     <row r="24">
       <c r="A24" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B24" s="12">
         <v>40.0</v>
@@ -13671,7 +13848,7 @@
     </row>
     <row r="26">
       <c r="A26" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B26" s="12">
         <v>30.0</v>
@@ -13682,7 +13859,7 @@
     </row>
     <row r="27">
       <c r="A27" s="12" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B27" s="12">
         <v>70.0</v>
@@ -13693,7 +13870,7 @@
     </row>
     <row r="28">
       <c r="A28" s="12" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B28" s="12">
         <v>80.0</v>
@@ -13704,7 +13881,7 @@
     </row>
     <row r="29">
       <c r="A29" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B29" s="12">
         <v>20.0</v>
@@ -13715,7 +13892,7 @@
     </row>
     <row r="30">
       <c r="A30" s="12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B30" s="12">
         <v>10.0</v>
@@ -13759,7 +13936,7 @@
     </row>
     <row r="34">
       <c r="A34" s="12" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B34" s="12">
         <v>55.0</v>
@@ -13770,7 +13947,7 @@
     </row>
     <row r="35">
       <c r="A35" s="12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B35" s="12">
         <v>4.0</v>
@@ -13814,7 +13991,7 @@
     </row>
     <row r="39">
       <c r="A39" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B39" s="12">
         <v>30.0</v>
@@ -13836,7 +14013,7 @@
     </row>
     <row r="41">
       <c r="A41" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B41" s="12">
         <v>33.0</v>
@@ -13847,7 +14024,7 @@
     </row>
     <row r="42">
       <c r="A42" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B42" s="12">
         <v>525.0</v>
@@ -13858,7 +14035,7 @@
     </row>
     <row r="43">
       <c r="A43" s="12" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B43" s="12">
         <v>55.0</v>
@@ -13869,7 +14046,7 @@
     </row>
     <row r="44">
       <c r="A44" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B44" s="12">
         <v>20.0</v>
@@ -13902,7 +14079,7 @@
     </row>
     <row r="47">
       <c r="A47" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B47" s="12">
         <v>40.0</v>
@@ -13924,7 +14101,7 @@
     </row>
     <row r="49">
       <c r="A49" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B49" s="12">
         <v>33.0</v>
@@ -13979,7 +14156,7 @@
     </row>
     <row r="54">
       <c r="A54" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B54" s="12">
         <v>33.0</v>
@@ -14012,7 +14189,7 @@
     </row>
     <row r="57">
       <c r="A57" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B57" s="12">
         <v>30.0</v>

</xml_diff>